<commit_message>
cambios en 21c por anual
</commit_message>
<xml_diff>
--- a/xlsx/a69_f21_cUPPachuca.xlsx
+++ b/xlsx/a69_f21_cUPPachuca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\Cierre Presupuestal Ene-Marz21\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lisbet\Documents\Dirección de Planeción\2021\SIPOT\Entrega SIPOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>46585</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>La información deberá incluir los estados financieros y demás información presupuestaria, programática y contable que emanen de los registros de los sujetos obligados; dichos estados deberán estar ordenados de conformidad con los criterios, lineamientos y disposiciones normativas correspondientes que emita el Consejo Nacional de Armonización Contable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La cuenta Públicas el ejercicio fiscal 2020, se entrega en la CACEH En marzo , motivo por el cual se indica el Hipervínculo </t>
   </si>
   <si>
     <t>http://www.upp.edu.mx/leygralcontabilidad/mc/03-cuenta_publica/01-caceh/2020/1-Acuse-de-recepcion-Cuenta-Publica-2020.aspx</t>
@@ -527,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,8 +539,8 @@
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="124" customWidth="1"/>
-    <col min="5" max="5" width="73.140625" customWidth="1"/>
+    <col min="4" max="4" width="98.7109375" customWidth="1"/>
+    <col min="5" max="5" width="73.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.7109375" customWidth="1"/>
@@ -673,7 +676,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2021</v>
       </c>
@@ -681,10 +684,10 @@
         <v>44197</v>
       </c>
       <c r="C8" s="4">
-        <v>44286</v>
+        <v>44561</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>29</v>
@@ -695,7 +698,9 @@
       <c r="G8" s="4">
         <v>44298</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>